<commit_message>
excel is updated IRT, added options for specific color and size
</commit_message>
<xml_diff>
--- a/angel.xlsx
+++ b/angel.xlsx
@@ -1,47 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\GitHub\Project-Angel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F718EE6-217D-471F-9340-1ADB66728544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FEB205-DAB9-4804-9AD3-C626F0062F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="2820" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2700" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>sku</t>
   </si>
   <si>
     <t>qty</t>
+  </si>
+  <si>
+    <t>ST-TS-1-DAWG-BLK-L</t>
+  </si>
+  <si>
+    <t>ST-TS-4-CRACK-GRN-M</t>
+  </si>
+  <si>
+    <t>ST-TS-6-HEART-WHT-L</t>
+  </si>
+  <si>
+    <t>ST-TS-1-DAWG-BLK-XL</t>
+  </si>
+  <si>
+    <t>ST-TS-5-YAP-BLK-XL</t>
+  </si>
+  <si>
+    <t>ST-TS-2-DAWG-GRN-XL</t>
+  </si>
+  <si>
+    <t>ST-TS-3-CRACK-BLK-L</t>
+  </si>
+  <si>
+    <t>ST-TS-6-HEART-WHT-XL</t>
   </si>
 </sst>
 </file>
@@ -77,9 +85,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -88,16 +99,16 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -113,14 +124,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F3AED98-7BFC-407D-8623-900DD75EFE70}" name="Table1" displayName="Table1" ref="A1:B8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B8" xr:uid="{4F3AED98-7BFC-407D-8623-900DD75EFE70}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E8BE38B4-A938-468B-8FAF-FB0462219F25}" name="sku" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{08D80734-2576-41E4-A80E-9D0FD0CAB3EF}" name="qty" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="sku" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="qty" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -443,16 +454,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,59 +475,67 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
+      <c r="A8" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small update for TS/HD selection
</commit_message>
<xml_diff>
--- a/angel.xlsx
+++ b/angel.xlsx
@@ -1,76 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\GitHub\Project-Angel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FEB205-DAB9-4804-9AD3-C626F0062F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2700" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="2700" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>qty</t>
-  </si>
-  <si>
-    <t>ST-TS-1-DAWG-BLK-L</t>
-  </si>
-  <si>
-    <t>ST-TS-4-CRACK-GRN-M</t>
-  </si>
-  <si>
-    <t>ST-TS-6-HEART-WHT-L</t>
-  </si>
-  <si>
-    <t>ST-TS-1-DAWG-BLK-XL</t>
-  </si>
-  <si>
-    <t>ST-TS-5-YAP-BLK-XL</t>
-  </si>
-  <si>
-    <t>ST-TS-2-DAWG-GRN-XL</t>
-  </si>
-  <si>
-    <t>ST-TS-3-CRACK-BLK-L</t>
-  </si>
-  <si>
-    <t>ST-TS-6-HEART-WHT-XL</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,12 +51,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -112,26 +81,83 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B10" headerRowCount="1" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B10"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="sku" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="qty" dataDxfId="0"/>
+    <tableColumn id="1" name="sku" dataDxfId="1"/>
+    <tableColumn id="2" name="qty" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -453,95 +479,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" customWidth="1"/>
+    <col width="22.140625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="8" customWidth="1" style="2" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>sku</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>qty</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-1-DAWG-BLK-L</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-4-CRACK-GRN-M</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-6-HEART-WHT-L</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-1-DAWG-BLK-XL</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-5-YAP-BLK-XL</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-2-DAWG-GRN-XL</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-3-CRACK-BLK-L</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>ST-TS-6-HEART-WHT-XL</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>ST-HD-7-DAWG-BLK-XL</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="n">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>